<commit_message>
update prix bapteme + excel
</commit_message>
<xml_diff>
--- a/assets/Coupon.xlsx
+++ b/assets/Coupon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cperr\Documents\GitHub\cresiracing\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casse\Documents\GitHub\cresiracing\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9895CD-213C-4F53-8C16-06B663983E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998B1913-6FBA-482B-B094-5154ADF995D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FCEF4C51-CCED-48A9-8810-D0B35A5EAEB0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCEF4C51-CCED-48A9-8810-D0B35A5EAEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Baptême</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Soit le total à payer (net) :</t>
+  </si>
+  <si>
+    <t>Coupon(s)</t>
+  </si>
+  <si>
+    <t>1 pour 5€</t>
+  </si>
+  <si>
+    <t>6 pour 30€</t>
   </si>
 </sst>
 </file>
@@ -179,7 +188,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -206,11 +218,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2A48DE0-1D2A-4B43-9C92-7C7BA1F63A73}" name="Tableau3" displayName="Tableau3" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B5" xr:uid="{D2A48DE0-1D2A-4B43-9C92-7C7BA1F63A73}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{278A3427-F213-4970-9844-513A3F64B22C}" name="Choix" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{89F890E3-CDA2-4990-890D-3EBF0AC1F141}" name="Combien de fois :" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2A48DE0-1D2A-4B43-9C92-7C7BA1F63A73}" name="Tableau3" displayName="Tableau3" ref="A1:C5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C5" xr:uid="{D2A48DE0-1D2A-4B43-9C92-7C7BA1F63A73}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{278A3427-F213-4970-9844-513A3F64B22C}" name="Choix" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{89F890E3-CDA2-4990-890D-3EBF0AC1F141}" name="Combien de fois :" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{3CCE1D49-AFAF-489F-BCB2-D98EB2BC3639}" name="Coupon(s)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -513,20 +526,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE8B1ED-7D60-4A6B-B9E4-7E6FF6C3D15A}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="3" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -534,47 +547,61 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -586,7 +613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -600,7 +627,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{8BFAAEDB-F68B-44DA-A953-350DF90FFA70}">
@@ -608,7 +635,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>